<commit_message>
Fixing up the modeling to get the factors right.
</commit_message>
<xml_diff>
--- a/Shadehouse/Biomass Experiment 1 Clean.xlsx
+++ b/Shadehouse/Biomass Experiment 1 Clean.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3dc651ccd8a4551c/Desktop/Thesis/Analysis/Multiple-Weeds-Impacts/Shadehouse/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1791" documentId="11_F25DC773A252ABDACC104868F99D74165BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0949528-6242-424B-991A-DFCB553923AA}"/>
+  <xr:revisionPtr revIDLastSave="1792" documentId="11_F25DC773A252ABDACC104868F99D74165BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5578234-7441-4B30-8077-66F4F8BAC4D1}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-8730" yWindow="-18225" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -181,16 +181,16 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,8 +474,8 @@
   <dimension ref="A1:Q1063"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <pane ySplit="1" topLeftCell="A803" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J823" sqref="J823"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -22938,7 +22938,7 @@
         <v>9</v>
       </c>
       <c r="J822" s="1">
-        <v>90</v>
+        <v>9</v>
       </c>
     </row>
     <row r="823" spans="1:10" x14ac:dyDescent="0.3">
@@ -28800,18 +28800,18 @@
   <conditionalFormatting sqref="C2:C341">
     <cfRule type="duplicateValues" priority="15"/>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D202:D245 D246:E294 D295:D301 E295:E345">
+    <cfRule type="duplicateValues" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D302:D341">
+    <cfRule type="duplicateValues" priority="4"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D2:E101">
     <cfRule type="duplicateValues" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D102:E198 D199:D201 E199:E245">
     <cfRule type="duplicateValues" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D202:D245 D246:E294 D295:D301 E295:E345">
-    <cfRule type="duplicateValues" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D302:D341">
-    <cfRule type="duplicateValues" priority="4"/>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>